<commit_message>
Update workout sample XLSX
</commit_message>
<xml_diff>
--- a/samples/Entrainement vélo elliptique3.xlsx
+++ b/samples/Entrainement vélo elliptique3.xlsx
@@ -17202,7 +17202,7 @@
         <v>64</v>
       </c>
       <c r="L20" s="14">
-        <f>IF(AND(ISNUMBER(I20),ISNUMBER(K20),K20&lt;&gt;0),15*I20/K20,"")</f>
+        <f t="shared" si="26"/>
         <v>32.8125</v>
       </c>
       <c r="M20" s="13">
@@ -17263,13 +17263,19 @@
         <f t="shared" si="26"/>
         <v>34.761904761904759</v>
       </c>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13" t="str">
+      <c r="M21" s="13">
+        <v>86</v>
+      </c>
+      <c r="N21" s="13">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-      <c r="O21" s="15"/>
-      <c r="P21" s="8"/>
+        <v>20.123999999999999</v>
+      </c>
+      <c r="O21" s="15">
+        <v>0.23399999999999999</v>
+      </c>
+      <c r="P21" s="8">
+        <v>103</v>
+      </c>
       <c r="Q21" s="8" t="s">
         <v>34</v>
       </c>
@@ -17277,7 +17283,7 @@
     </row>
     <row r="22" ht="14.25">
       <c r="A22" s="12">
-        <v>46043</v>
+        <v>46043.260416666664</v>
       </c>
       <c r="B22" s="8">
         <v>4444444444</v>
@@ -17285,37 +17291,57 @@
       <c r="C22" s="8">
         <v>45</v>
       </c>
-      <c r="D22" s="9" t="str">
+      <c r="D22" s="9">
         <f t="shared" si="24"/>
-        <v/>
-      </c>
-      <c r="E22" s="13"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="13" t="str">
+        <v>12.533333333333335</v>
+      </c>
+      <c r="E22" s="13">
+        <v>9.4000000000000004</v>
+      </c>
+      <c r="F22" s="8">
+        <v>730</v>
+      </c>
+      <c r="G22" s="13">
         <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="14" t="str">
+        <v>77.659574468085097</v>
+      </c>
+      <c r="H22" s="8">
+        <v>119</v>
+      </c>
+      <c r="I22" s="8">
+        <v>132</v>
+      </c>
+      <c r="J22" s="8">
+        <v>80</v>
+      </c>
+      <c r="K22" s="8">
+        <v>62</v>
+      </c>
+      <c r="L22" s="14">
         <f t="shared" si="26"/>
-        <v/>
-      </c>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13" t="str">
+        <v>31.93548387096774</v>
+      </c>
+      <c r="M22" s="13">
+        <v>86.299999999999997</v>
+      </c>
+      <c r="N22" s="13">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-      <c r="O22" s="15"/>
-      <c r="P22" s="8"/>
-      <c r="Q22" s="8"/>
+        <v>19.935300000000002</v>
+      </c>
+      <c r="O22" s="15">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="P22" s="8">
+        <v>103</v>
+      </c>
+      <c r="Q22" s="8" t="s">
+        <v>34</v>
+      </c>
       <c r="R22" s="8"/>
     </row>
     <row r="23" ht="14.25">
       <c r="A23" s="12">
-        <v>46044</v>
+        <v>46044.25</v>
       </c>
       <c r="B23" s="8">
         <v>4444444444</v>
@@ -17323,32 +17349,52 @@
       <c r="C23" s="8">
         <v>45</v>
       </c>
-      <c r="D23" s="9" t="str">
+      <c r="D23" s="9">
         <f t="shared" si="24"/>
-        <v/>
-      </c>
-      <c r="E23" s="13"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="13" t="str">
+        <v>12.400000000000002</v>
+      </c>
+      <c r="E23" s="13">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="F23" s="8">
+        <v>728</v>
+      </c>
+      <c r="G23" s="13">
         <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="14" t="str">
+        <v>78.279569892473106</v>
+      </c>
+      <c r="H23" s="8">
+        <v>121</v>
+      </c>
+      <c r="I23" s="8">
+        <v>133</v>
+      </c>
+      <c r="J23" s="8">
+        <v>103</v>
+      </c>
+      <c r="K23" s="8">
+        <v>69</v>
+      </c>
+      <c r="L23" s="14">
         <f t="shared" si="26"/>
-        <v/>
-      </c>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13" t="str">
+        <v>28.913043478260871</v>
+      </c>
+      <c r="M23" s="13">
+        <v>86.5</v>
+      </c>
+      <c r="N23" s="13">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-      <c r="O23" s="15"/>
-      <c r="P23" s="8"/>
-      <c r="Q23" s="8"/>
+        <v>20.414000000000001</v>
+      </c>
+      <c r="O23" s="15">
+        <v>0.23600000000000002</v>
+      </c>
+      <c r="P23" s="8">
+        <v>103</v>
+      </c>
+      <c r="Q23" s="8" t="s">
+        <v>34</v>
+      </c>
       <c r="R23" s="8"/>
     </row>
     <row r="24" ht="14.25">

</xml_diff>